<commit_message>
fixed some null values
</commit_message>
<xml_diff>
--- a/project-files/datasets/original/project_data/211_Info_Data_compiled-excel.xlsx
+++ b/project-files/datasets/original/project_data/211_Info_Data_compiled-excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steph\local\oit-class\project-files\datasets\original\project_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7485F1E6-3128-4B52-A483-3D502006D53F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0156B20B-4083-42E8-8C98-D3223AD1DA2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-72" yWindow="0" windowWidth="23112" windowHeight="12120" xr2:uid="{5DA4BD90-C6F9-4E22-B2F0-02384526907D}"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="23040" windowHeight="12120" xr2:uid="{5DA4BD90-C6F9-4E22-B2F0-02384526907D}"/>
   </bookViews>
   <sheets>
     <sheet name="list" sheetId="12" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="250">
   <si>
     <t>Resource Name</t>
   </si>
@@ -1060,7 +1060,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="52">
+  <dxfs count="53">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1142,728 +1142,14 @@
       </fill>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -2006,6 +1292,730 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2019,19 +2029,15 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{99D87425-83CA-48AE-96AE-243E809B78F6}" name="Table1" displayName="Table1" ref="B1:F15" totalsRowShown="0">
   <autoFilter ref="B1:F15" xr:uid="{99D87425-83CA-48AE-96AE-243E809B78F6}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{B4EED3DD-8B29-4FD2-9209-155CE9A4422E}" name="Resource Name" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{524B6E03-0488-444D-8A97-782B6B94F931}" name="Address" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{D8A63C3A-1A0E-4A84-8483-4FD26C90477C}" name="Zip" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{925A60A5-9F5C-4E86-B346-4F9CFD693CB6}" name="Hours" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{89C8D6F5-9ED0-4126-91F0-BB2EDDD36B59}" name="Description" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{B4EED3DD-8B29-4FD2-9209-155CE9A4422E}" name="Resource Name" dataDxfId="52"/>
+    <tableColumn id="2" xr3:uid="{524B6E03-0488-444D-8A97-782B6B94F931}" name="Address" dataDxfId="51"/>
+    <tableColumn id="4" xr3:uid="{D8A63C3A-1A0E-4A84-8483-4FD26C90477C}" name="Zip" dataDxfId="50"/>
+    <tableColumn id="5" xr3:uid="{925A60A5-9F5C-4E86-B346-4F9CFD693CB6}" name="Hours" dataDxfId="49"/>
+    <tableColumn id="6" xr3:uid="{89C8D6F5-9ED0-4126-91F0-BB2EDDD36B59}" name="Description" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2041,11 +2047,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{AC896013-CAEA-40AE-94DD-CB5C3D09391B}" name="Table24" displayName="Table24" ref="B1:F6" totalsRowShown="0">
   <autoFilter ref="B1:F6" xr:uid="{AC896013-CAEA-40AE-94DD-CB5C3D09391B}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{EE4F3B92-E3B1-4816-9045-9978EDC9C71A}" name="Resource Name" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{3F9DAFA9-C864-401D-A37A-60A607D7F4DC}" name="Address" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{974641C0-B601-4418-97FE-C944C49AB2B0}" name="Zip" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{148F5EBA-63E0-43AF-8F65-D6C5EB616306}" name="Hours" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{D4199F39-819C-4485-93B3-5047FEBDA570}" name="Description" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{EE4F3B92-E3B1-4816-9045-9978EDC9C71A}" name="Resource Name" dataDxfId="47"/>
+    <tableColumn id="2" xr3:uid="{3F9DAFA9-C864-401D-A37A-60A607D7F4DC}" name="Address" dataDxfId="46"/>
+    <tableColumn id="3" xr3:uid="{974641C0-B601-4418-97FE-C944C49AB2B0}" name="Zip" dataDxfId="45"/>
+    <tableColumn id="4" xr3:uid="{148F5EBA-63E0-43AF-8F65-D6C5EB616306}" name="Hours" dataDxfId="44"/>
+    <tableColumn id="5" xr3:uid="{D4199F39-819C-4485-93B3-5047FEBDA570}" name="Description" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2055,25 +2061,25 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C51A409A-CB35-4A49-9CF1-54EC4120F608}" name="Table2" displayName="Table2" ref="B1:F11" totalsRowShown="0">
   <autoFilter ref="B1:F11" xr:uid="{C51A409A-CB35-4A49-9CF1-54EC4120F608}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{9D3669AA-13F6-4BE5-9946-40DC23163CB2}" name="Resource Name" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{E06D1DFC-F039-4004-9BA8-8202A97EC864}" name="Address" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{779ED0F5-A46F-4251-AE45-FADEB92CE293}" name="Zip" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{CF5C985A-0623-41C9-8A2D-AD2E2F73C4D9}" name="Hours" dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{892FD4E3-0372-4E11-BBCE-34A5CAA7B46A}" name="Description" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{9D3669AA-13F6-4BE5-9946-40DC23163CB2}" name="Resource Name" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{E06D1DFC-F039-4004-9BA8-8202A97EC864}" name="Address" dataDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{779ED0F5-A46F-4251-AE45-FADEB92CE293}" name="Zip" dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{CF5C985A-0623-41C9-8A2D-AD2E2F73C4D9}" name="Hours" dataDxfId="39"/>
+    <tableColumn id="5" xr3:uid="{892FD4E3-0372-4E11-BBCE-34A5CAA7B46A}" name="Description" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{0876AC89-3A31-4CFE-9405-5F75FFABC868}" name="Table2567" displayName="Table2567" ref="A1:E17" totalsRowShown="0" headerRowDxfId="42" headerRowBorderDxfId="41" tableBorderDxfId="40" totalsRowBorderDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{0876AC89-3A31-4CFE-9405-5F75FFABC868}" name="Table2567" displayName="Table2567" ref="A1:E17" totalsRowShown="0" headerRowDxfId="37" headerRowBorderDxfId="36" tableBorderDxfId="35" totalsRowBorderDxfId="34">
   <autoFilter ref="A1:E17" xr:uid="{C51A409A-CB35-4A49-9CF1-54EC4120F608}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{F9D2CEC8-654C-4FE3-B970-E48E4E7ACBD4}" name="Resource Name" dataDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{D0BDDC8C-C0B5-45A5-8BE9-29C5FE648495}" name="Address" dataDxfId="37"/>
-    <tableColumn id="6" xr3:uid="{92AF2AC0-0444-4827-B864-2BC055C000B5}" name="Zip" dataDxfId="36"/>
-    <tableColumn id="7" xr3:uid="{746986AB-924E-45BD-8D50-26DAC6F26AB7}" name="Column1" dataDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{A2470039-126E-4A5F-AE23-5F4562EBEF08}" name="library" dataDxfId="34"/>
+    <tableColumn id="1" xr3:uid="{F9D2CEC8-654C-4FE3-B970-E48E4E7ACBD4}" name="Resource Name" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{D0BDDC8C-C0B5-45A5-8BE9-29C5FE648495}" name="Address" dataDxfId="32"/>
+    <tableColumn id="6" xr3:uid="{92AF2AC0-0444-4827-B864-2BC055C000B5}" name="Zip" dataDxfId="31"/>
+    <tableColumn id="7" xr3:uid="{746986AB-924E-45BD-8D50-26DAC6F26AB7}" name="Column1" dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{A2470039-126E-4A5F-AE23-5F4562EBEF08}" name="library" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2083,12 +2089,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6DA4DB0A-D95D-4F8E-9B21-327BFB03C9D0}" name="Table256" displayName="Table256" ref="B1:G17" totalsRowShown="0">
   <autoFilter ref="B1:G17" xr:uid="{C51A409A-CB35-4A49-9CF1-54EC4120F608}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{6C3925CB-400B-4F9F-ACAB-C277CEAEBD08}" name="Resource Name" dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{E9B03D1E-595B-4F1C-AC2E-187C62E06BE9}" name="Address" dataDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{41E3025F-3276-4A92-9FD1-5309F862EC18}" name="Zip" dataDxfId="31"/>
-    <tableColumn id="4" xr3:uid="{96C8CF05-B5CE-4C72-BDE5-3FDA67EB8C3D}" name="Hours" dataDxfId="30"/>
-    <tableColumn id="6" xr3:uid="{1E04CDA0-9F91-4CD9-9895-2ECBB870AF0A}" name="showers" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{A9368E5C-82F7-4F4C-83F5-4D1661C1F7D8}" name="Description" dataDxfId="29"/>
+    <tableColumn id="1" xr3:uid="{6C3925CB-400B-4F9F-ACAB-C277CEAEBD08}" name="Resource Name" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{E9B03D1E-595B-4F1C-AC2E-187C62E06BE9}" name="Address" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{41E3025F-3276-4A92-9FD1-5309F862EC18}" name="Zip" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{96C8CF05-B5CE-4C72-BDE5-3FDA67EB8C3D}" name="Hours" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{1E04CDA0-9F91-4CD9-9895-2ECBB870AF0A}" name="showers" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{A9368E5C-82F7-4F4C-83F5-4D1661C1F7D8}" name="Description" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2098,24 +2104,24 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E95B0D76-3ACF-4E03-8965-362FB67FE615}" name="Table25" displayName="Table25" ref="A1:E5" totalsRowShown="0">
   <autoFilter ref="A1:E5" xr:uid="{C51A409A-CB35-4A49-9CF1-54EC4120F608}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{76DE051A-D9F9-4978-AC96-511F83477935}" name="Resource Name" dataDxfId="28"/>
-    <tableColumn id="2" xr3:uid="{15AF4591-2906-4F22-B7BC-E7D4F3E75AF7}" name="Address" dataDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{A25323DD-51C8-4524-978F-E683830FCAB1}" name="Zip" dataDxfId="26"/>
-    <tableColumn id="4" xr3:uid="{F7AEEA44-FA48-4830-BA5E-3A0016192A13}" name="Hours" dataDxfId="25"/>
-    <tableColumn id="5" xr3:uid="{7A2311B8-F2C4-4211-8EA4-1E1B87002BF3}" name="Description" dataDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{76DE051A-D9F9-4978-AC96-511F83477935}" name="Resource Name" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{15AF4591-2906-4F22-B7BC-E7D4F3E75AF7}" name="Address" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{A25323DD-51C8-4524-978F-E683830FCAB1}" name="Zip" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{F7AEEA44-FA48-4830-BA5E-3A0016192A13}" name="Hours" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{7A2311B8-F2C4-4211-8EA4-1E1B87002BF3}" name="Description" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{053FD1F8-B8D9-44DE-A1D0-EBFAD920AD43}" name="Table7" displayName="Table7" ref="A1:D61" totalsRowShown="0" headerRowDxfId="51" dataDxfId="49" headerRowBorderDxfId="50" tableBorderDxfId="48" totalsRowBorderDxfId="47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{053FD1F8-B8D9-44DE-A1D0-EBFAD920AD43}" name="Table7" displayName="Table7" ref="A1:D61" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
   <autoFilter ref="A1:D61" xr:uid="{053FD1F8-B8D9-44DE-A1D0-EBFAD920AD43}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{ED2CEAB5-6990-4B6D-9BCC-93F47872F79A}" name="Resource Name" dataDxfId="46"/>
-    <tableColumn id="2" xr3:uid="{EBC783BD-0A41-4D11-9B45-22DCB8F5ABD2}" name="Address" dataDxfId="45"/>
-    <tableColumn id="3" xr3:uid="{8E53413A-069D-4746-AC33-91F712F94CBF}" name="Zip" dataDxfId="44"/>
-    <tableColumn id="4" xr3:uid="{A4ACA6F0-C3A4-4B9F-826A-F395292FA57F}" name="Resource Tab Topics " dataDxfId="43"/>
+    <tableColumn id="1" xr3:uid="{ED2CEAB5-6990-4B6D-9BCC-93F47872F79A}" name="Resource Name" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{EBC783BD-0A41-4D11-9B45-22DCB8F5ABD2}" name="Address" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{8E53413A-069D-4746-AC33-91F712F94CBF}" name="Zip" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{A4ACA6F0-C3A4-4B9F-826A-F395292FA57F}" name="Resource Tab Topics " dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium28" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2440,9 +2446,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{191AC4CA-521B-478C-853D-4192550E2637}">
   <dimension ref="A1:R65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T16" sqref="T16"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2526,6 +2532,9 @@
       <c r="C2">
         <v>97212</v>
       </c>
+      <c r="D2" t="s">
+        <v>249</v>
+      </c>
       <c r="E2" s="17">
         <v>1</v>
       </c>
@@ -2579,6 +2588,9 @@
       <c r="C3">
         <v>97219</v>
       </c>
+      <c r="D3" t="s">
+        <v>249</v>
+      </c>
       <c r="E3" s="17">
         <v>1</v>
       </c>
@@ -2632,6 +2644,9 @@
       <c r="C4">
         <v>97205</v>
       </c>
+      <c r="D4" t="s">
+        <v>249</v>
+      </c>
       <c r="E4" s="17">
         <v>1</v>
       </c>
@@ -2685,6 +2700,9 @@
       <c r="C5">
         <v>97213</v>
       </c>
+      <c r="D5" t="s">
+        <v>249</v>
+      </c>
       <c r="E5" s="17">
         <v>1</v>
       </c>
@@ -2738,6 +2756,9 @@
       <c r="C6">
         <v>97239</v>
       </c>
+      <c r="D6" t="s">
+        <v>249</v>
+      </c>
       <c r="E6" s="17">
         <v>1</v>
       </c>
@@ -2791,6 +2812,9 @@
       <c r="C7">
         <v>97206</v>
       </c>
+      <c r="D7" t="s">
+        <v>249</v>
+      </c>
       <c r="E7" s="17">
         <v>1</v>
       </c>
@@ -2844,6 +2868,9 @@
       <c r="C8">
         <v>97217</v>
       </c>
+      <c r="D8" t="s">
+        <v>249</v>
+      </c>
       <c r="E8" s="17">
         <v>1</v>
       </c>
@@ -2897,6 +2924,9 @@
       <c r="C9">
         <v>97233</v>
       </c>
+      <c r="D9" t="s">
+        <v>249</v>
+      </c>
       <c r="E9" s="17">
         <v>1</v>
       </c>
@@ -2950,6 +2980,9 @@
       <c r="C10">
         <v>97217</v>
       </c>
+      <c r="D10" t="s">
+        <v>249</v>
+      </c>
       <c r="E10" s="17">
         <v>1</v>
       </c>
@@ -3003,6 +3036,9 @@
       <c r="C11">
         <v>97210</v>
       </c>
+      <c r="D11" t="s">
+        <v>249</v>
+      </c>
       <c r="E11" s="17">
         <v>1</v>
       </c>
@@ -3056,6 +3092,9 @@
       <c r="C12">
         <v>97214</v>
       </c>
+      <c r="D12" t="s">
+        <v>249</v>
+      </c>
       <c r="E12" s="17">
         <v>1</v>
       </c>
@@ -3109,6 +3148,9 @@
       <c r="C13">
         <v>97212</v>
       </c>
+      <c r="D13" t="s">
+        <v>249</v>
+      </c>
       <c r="E13" s="17">
         <v>1</v>
       </c>
@@ -3162,6 +3204,9 @@
       <c r="C14">
         <v>97233</v>
       </c>
+      <c r="D14" t="s">
+        <v>249</v>
+      </c>
       <c r="E14" s="17">
         <v>1</v>
       </c>
@@ -3215,6 +3260,9 @@
       <c r="C15">
         <v>97202</v>
       </c>
+      <c r="D15" t="s">
+        <v>249</v>
+      </c>
       <c r="E15" s="17">
         <v>1</v>
       </c>
@@ -3268,6 +3316,9 @@
       <c r="C16">
         <v>97203</v>
       </c>
+      <c r="D16" t="s">
+        <v>249</v>
+      </c>
       <c r="E16" s="17">
         <v>1</v>
       </c>
@@ -3321,6 +3372,9 @@
       <c r="C17">
         <v>97206</v>
       </c>
+      <c r="D17" t="s">
+        <v>249</v>
+      </c>
       <c r="E17" s="17">
         <v>1</v>
       </c>
@@ -6000,6 +6054,15 @@
       <c r="A65" t="s">
         <v>239</v>
       </c>
+      <c r="B65" t="s">
+        <v>119</v>
+      </c>
+      <c r="C65">
+        <v>97233</v>
+      </c>
+      <c r="D65" t="s">
+        <v>176</v>
+      </c>
       <c r="E65" s="17">
         <v>0</v>
       </c>
@@ -6044,11 +6107,11 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B11 B12:D17">
-    <cfRule type="duplicateValues" dxfId="7" priority="2"/>
+  <conditionalFormatting sqref="B2:B11 B12:C17">
+    <cfRule type="duplicateValues" dxfId="8" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:B32">
-    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6466,7 +6529,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -6947,7 +7010,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -7275,7 +7338,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B11 B12:C17">
-    <cfRule type="duplicateValues" dxfId="3" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -7699,7 +7762,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="str">
-        <f t="shared" ref="A20:B35" si="1">PROPER(B20)</f>
+        <f t="shared" ref="A20:A33" si="1">PROPER(B20)</f>
         <v/>
       </c>
     </row>
@@ -7832,7 +7895,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B36" t="str">
-        <f t="shared" ref="B28:B41" si="2">PROPER(C36)</f>
+        <f t="shared" ref="B36:B41" si="2">PROPER(C36)</f>
         <v/>
       </c>
     </row>
@@ -7868,7 +7931,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C17">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -8862,10 +8925,10 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B11 B12:C17">
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>